<commit_message>
initialise the table with 1 instead of 0
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -622,15 +622,59 @@
     </r>
   </si>
   <si>
-    <t>spam:</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>normal:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>This is wrong, need to separate attr_0, true, spam/normal</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ormal:</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -669,12 +713,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -704,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -712,8 +762,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1063,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R201"/>
+  <dimension ref="A1:W201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1079,10 +1132,15 @@
     <col min="16" max="16" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.25" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="1"/>
+    <col min="19" max="19" width="1.75" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1163,11 +1221,8 @@
       <c r="M2" s="2">
         <v>1</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1207,682 +1262,867 @@
       <c r="M3" s="2">
         <v>1</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="2">
-        <f>COUNTIF(A2:A201,1)</f>
-        <v>87</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R3" s="2">
-        <f>COUNTIF(A2:A201,0)</f>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="2">
-        <f>COUNTIF(B2:B201,1)</f>
-        <v>116</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="2">
-        <f>COUNTIF(B2:B201,0)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="2">
-        <f>COUNTIF(C2:C201,1)</f>
-        <v>74</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R5" s="2">
-        <f>COUNTIF(C2:C201,0)</f>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="2">
-        <f>COUNTIF(D2:D201,1)</f>
-        <v>90</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" s="2">
-        <f>COUNTIF(D2:D201,0)</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" s="2">
-        <f>COUNTIF(E2:E201,1)</f>
-        <v>75</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="2">
-        <f>COUNTIF(E2:E201,0)</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="2">
-        <f>COUNTIF(F2:F201,1)</f>
-        <v>88</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8" s="2">
-        <f>COUNTIF(F2:F201,0)</f>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="2">
-        <f>COUNTIF(G2:G201,1)</f>
-        <v>115</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R9" s="2">
-        <f>COUNTIF(G2:G201,0)</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P10" s="2">
-        <f>COUNTIF(H2:H201,1)</f>
-        <v>91</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R10" s="2">
-        <f>COUNTIF(H2:H201,0)</f>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2">
-        <v>1</v>
-      </c>
-      <c r="M11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P11" s="2">
-        <f>COUNTIF(I2:I201,1)</f>
-        <v>53</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="2">
-        <f>COUNTIF(I2:I201,0)</f>
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P12" s="2">
-        <f>COUNTIF(J2:J201,1)</f>
-        <v>77</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R12" s="2">
-        <f>COUNTIF(J2:J201,0)</f>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" s="2">
-        <f>COUNTIF(K2:K201,1)</f>
-        <v>121</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R13" s="2">
-        <f>COUNTIF(K2:K201,0)</f>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" s="2">
-        <f>COUNTIF(L2:L201,1)</f>
-        <v>90</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R14" s="2">
-        <f>COUNTIF(L2:L201,0)</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-      <c r="M15" s="2">
-        <v>1</v>
-      </c>
-      <c r="O15" s="2" t="s">
+      <c r="O3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3">
         <f>COUNTIF(M2:M201,1)</f>
         <v>51</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="R3" s="3"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="R15" s="2">
+      <c r="U3" s="3"/>
+      <c r="V3" s="3">
         <f>COUNTIF(M2:M201,0)</f>
         <v>149</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="2">
+        <f>COUNTIF(A2:A52,1)</f>
+        <v>34</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="2">
+        <f>COUNTIF(A2:A52,0)</f>
+        <v>17</v>
+      </c>
+      <c r="S4" s="4"/>
+      <c r="T4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="2">
+        <f>COUNTIF(A53:A201,1)</f>
+        <v>53</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W4" s="2">
+        <f>COUNTIF(A53:A201,0)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="2">
+        <f>COUNTIF(B2:B52,1)</f>
+        <v>30</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="2">
+        <f>COUNTIF(B2:B52,0)</f>
+        <v>21</v>
+      </c>
+      <c r="S5" s="4"/>
+      <c r="T5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="2">
+        <f>COUNTIF(B53:B201,1)</f>
+        <v>86</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="2">
+        <f>COUNTIF(B53:B201,0)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6" s="2">
+        <f>COUNTIF(C2:C52,1)</f>
+        <v>23</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R6" s="2">
+        <f>COUNTIF(C2:C52,0)</f>
+        <v>28</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="2">
+        <f>COUNTIF(C53:C201,1)</f>
+        <v>51</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="2">
+        <f>COUNTIF(C53:C201,0)</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="2">
+        <f>COUNTIF(D2:D52,1)</f>
+        <v>31</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="2">
+        <f>COUNTIF(D2:D52,0)</f>
+        <v>20</v>
+      </c>
+      <c r="S7" s="4"/>
+      <c r="T7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="2">
+        <f>COUNTIF(D53:D201,1)</f>
+        <v>59</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7" s="2">
+        <f>COUNTIF(D53:D201,0)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="2">
+        <f>COUNTIF(E2:E52,1)</f>
+        <v>25</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="2">
+        <f>COUNTIF(E2:E52,0)</f>
+        <v>26</v>
+      </c>
+      <c r="S8" s="4"/>
+      <c r="T8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U8" s="2">
+        <f>COUNTIF(E53:E201,1)</f>
+        <v>50</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W8" s="2">
+        <f>COUNTIF(E53:E201,0)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="2">
+        <f>COUNTIF(F2:F52,1)</f>
+        <v>18</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="2">
+        <f>COUNTIF(F2:F52,0)</f>
+        <v>33</v>
+      </c>
+      <c r="S9" s="4"/>
+      <c r="T9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" s="2">
+        <f>COUNTIF(F53:F201,1)</f>
+        <v>70</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="W9" s="2">
+        <f>COUNTIF(F53:F201,0)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="2">
+        <f>COUNTIF(G2:G52,1)</f>
+        <v>40</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" s="2">
+        <f>COUNTIF(G2:G52,0)</f>
+        <v>11</v>
+      </c>
+      <c r="S10" s="4"/>
+      <c r="T10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="2">
+        <f>COUNTIF(G53:G201,1)</f>
+        <v>75</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W10" s="2">
+        <f>COUNTIF(G53:G201,0)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="2">
+        <f>COUNTIF(H2:H52,1)</f>
+        <v>39</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="2">
+        <f>COUNTIF(H2:H52,0)</f>
+        <v>12</v>
+      </c>
+      <c r="S11" s="4"/>
+      <c r="T11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="2">
+        <f>COUNTIF(H53:H201,1)</f>
+        <v>52</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" s="2">
+        <f>COUNTIF(H53:H201,0)</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="2">
+        <f>COUNTIF(I2:I52,1)</f>
+        <v>17</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" s="2">
+        <f>COUNTIF(I2:I52,0)</f>
+        <v>34</v>
+      </c>
+      <c r="S12" s="4"/>
+      <c r="T12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="2">
+        <f>COUNTIF(I53:I201,1)</f>
+        <v>36</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W12" s="2">
+        <f>COUNTIF(I53:I201,0)</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="2">
+        <f>COUNTIF(J2:J52,1)</f>
+        <v>34</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" s="2">
+        <f>COUNTIF(J2:J52,0)</f>
+        <v>17</v>
+      </c>
+      <c r="S13" s="4"/>
+      <c r="T13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13" s="2">
+        <f>COUNTIF(J53:J201,1)</f>
+        <v>43</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13" s="2">
+        <f>COUNTIF(J53:J201,0)</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" s="2">
+        <f>COUNTIF(K2:K52,1)</f>
+        <v>34</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" s="2">
+        <f>COUNTIF(K2:K52,0)</f>
+        <v>17</v>
+      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U14" s="2">
+        <f>COUNTIF(K53:K201,1)</f>
+        <v>87</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14" s="2">
+        <f>COUNTIF(K53:K201,0)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" s="2">
+        <f>COUNTIF(L2:L52,1)</f>
+        <v>40</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" s="2">
+        <f>COUNTIF(L2:L52,0)</f>
+        <v>11</v>
+      </c>
+      <c r="S15" s="4"/>
+      <c r="T15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U15" s="2">
+        <f>COUNTIF(L53:L201,1)</f>
+        <v>50</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W15" s="2">
+        <f>COUNTIF(L53:L201,0)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>0</v>
       </c>
@@ -1922,6 +2162,15 @@
       <c r="M16" s="2">
         <v>1</v>
       </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
@@ -9509,6 +9758,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update the excel table
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <r>
       <rPr>
@@ -41,7 +41,7 @@
       </rPr>
       <t>0</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -64,7 +64,7 @@
       </rPr>
       <t>1</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -417,272 +417,152 @@
       </rPr>
       <t>abel</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>attr_0, true:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>false</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">attr_0, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>false</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>false</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>attr_1, true:</t>
+    <t>true</t>
   </si>
   <si>
-    <t>attr_2, true:</t>
+    <t>true</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>attr_3, true:</t>
+    <t>attr_0</t>
   </si>
   <si>
-    <t>attr_4, true:</t>
+    <t>attr_0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>attr_5, true:</t>
+    <t>attr_1</t>
   </si>
   <si>
-    <t>attr_6, true:</t>
+    <t>attr_1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>attr_7, true:</t>
+    <t>attr_2</t>
   </si>
   <si>
-    <t>attr_8, true:</t>
+    <t>attr_2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>attr_9, true:</t>
+    <t>attr_3</t>
   </si>
   <si>
-    <t>attr_10, true:</t>
+    <t>attr_3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>attr_11, true:</t>
+    <t>attr_4</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_1, false:</t>
-    </r>
+    <t>attr_4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_2, false:</t>
-    </r>
+    <t>attr_5</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_3, false:</t>
-    </r>
+    <t>attr_5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_4, false:</t>
-    </r>
+    <t>attr_6</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_5, false:</t>
-    </r>
+    <t>attr_6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_6, false:</t>
-    </r>
+    <t>attr_7</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_7, false:</t>
-    </r>
+    <t>attr_7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_8, false:</t>
-    </r>
+    <t>attr_8</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_9, false:</t>
-    </r>
+    <t>attr_8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_10, false:</t>
-    </r>
+    <t>attr_9</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attr_11, false:</t>
-    </r>
+    <t>attr_9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>attr_10</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ormal:</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <t>attr_10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>attr_11</t>
+  </si>
+  <si>
+    <t>attr_11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spam</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>normal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>probability</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>class probability</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>occurrence</t>
+  </si>
+  <si>
+    <t>occurrence</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total occurrence</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -699,13 +579,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
@@ -713,21 +586,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -750,11 +617,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -765,7 +706,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1116,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W201"/>
+  <dimension ref="A1:AE201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T26" sqref="T26"/>
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1128,19 +1123,26 @@
     <col min="11" max="12" width="7.125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="1.75" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9" style="1"/>
+    <col min="15" max="15" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="9" style="1"/>
+    <col min="26" max="26" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1180,8 +1182,21 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="O1" s="12"/>
+      <c r="P1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1221,8 +1236,37 @@
       <c r="M2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="O2" s="13"/>
+      <c r="P2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="10"/>
+      <c r="T2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="10"/>
+      <c r="V2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="10"/>
+      <c r="Z2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE2" s="8"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1262,1573 +1306,2179 @@
       <c r="M3" s="2">
         <v>1</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="11"/>
+      <c r="P3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="3">
+        <f>COUNTIF(A2:A52,1)+1</f>
+        <v>35</v>
+      </c>
+      <c r="Q4" s="14">
+        <f>P4/(P4+R4)</f>
+        <v>0.660377358490566</v>
+      </c>
+      <c r="R4" s="3">
+        <f>COUNTIF(A2:A52,0)+1</f>
+        <v>18</v>
+      </c>
+      <c r="S4" s="14">
+        <f>R4/(P4+R4)</f>
+        <v>0.33962264150943394</v>
+      </c>
+      <c r="T4" s="3">
+        <f>COUNTIF(A53:A201,1)+1</f>
+        <v>54</v>
+      </c>
+      <c r="U4" s="14">
+        <f>T4/(T4+V4)</f>
+        <v>0.35761589403973509</v>
+      </c>
+      <c r="V4" s="3">
+        <f>COUNTIF(A53:A201,0)+1</f>
+        <v>97</v>
+      </c>
+      <c r="W4" s="14">
+        <f>V4/(T4+V4)</f>
+        <v>0.64238410596026485</v>
+      </c>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>35</v>
+      </c>
+      <c r="AC4" s="14">
+        <v>0.660377358490566</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>18</v>
+      </c>
+      <c r="AE4" s="14">
+        <v>0.33962264150943394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="3">
+        <f>COUNTIF(B2:B52,1)+1</f>
+        <v>31</v>
+      </c>
+      <c r="Q5" s="14">
+        <f t="shared" ref="Q5:Q15" si="0">P5/(P5+R5)</f>
+        <v>0.58490566037735847</v>
+      </c>
+      <c r="R5" s="3">
+        <f>COUNTIF(B2:B52,0)+1</f>
+        <v>22</v>
+      </c>
+      <c r="S5" s="14">
+        <f t="shared" ref="S5:S15" si="1">R5/(P5+R5)</f>
+        <v>0.41509433962264153</v>
+      </c>
+      <c r="T5" s="3">
+        <f>COUNTIF(B53:B201,1)+1</f>
+        <v>87</v>
+      </c>
+      <c r="U5" s="14">
+        <f t="shared" ref="U5:U15" si="2">T5/(T5+V5)</f>
+        <v>0.57615894039735094</v>
+      </c>
+      <c r="V5" s="3">
+        <f>COUNTIF(B53:B201,0)+1</f>
+        <v>64</v>
+      </c>
+      <c r="W5" s="14">
+        <f t="shared" ref="W5:W15" si="3">V5/(T5+V5)</f>
+        <v>0.42384105960264901</v>
+      </c>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>31</v>
+      </c>
+      <c r="AC5" s="14">
+        <v>0.58490566037735847</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>22</v>
+      </c>
+      <c r="AE5" s="14">
+        <v>0.41509433962264153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="3">
+        <f>COUNTIF(C2:C52,1)+1</f>
+        <v>24</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.45283018867924529</v>
+      </c>
+      <c r="R6" s="3">
+        <f>COUNTIF(C2:C52,0)+1</f>
+        <v>29</v>
+      </c>
+      <c r="S6" s="14">
+        <f t="shared" si="1"/>
+        <v>0.54716981132075471</v>
+      </c>
+      <c r="T6" s="3">
+        <f>COUNTIF(C53:C201,1)+1</f>
+        <v>52</v>
+      </c>
+      <c r="U6" s="14">
+        <f t="shared" si="2"/>
+        <v>0.3443708609271523</v>
+      </c>
+      <c r="V6" s="3">
+        <f>COUNTIF(C53:C201,0)+1</f>
+        <v>99</v>
+      </c>
+      <c r="W6" s="14">
+        <f t="shared" si="3"/>
+        <v>0.6556291390728477</v>
+      </c>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>24</v>
+      </c>
+      <c r="AC6" s="14">
+        <v>0.45283018867924529</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>29</v>
+      </c>
+      <c r="AE6" s="14">
+        <v>0.54716981132075471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="3">
+        <f>COUNTIF(D2:D52,1)+1</f>
+        <v>32</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="0"/>
+        <v>0.60377358490566035</v>
+      </c>
+      <c r="R7" s="3">
+        <f>COUNTIF(D2:D52,0)+1</f>
+        <v>21</v>
+      </c>
+      <c r="S7" s="14">
+        <f t="shared" si="1"/>
+        <v>0.39622641509433965</v>
+      </c>
+      <c r="T7" s="3">
+        <f>COUNTIF(D53:D201,1)+1</f>
+        <v>60</v>
+      </c>
+      <c r="U7" s="14">
+        <f t="shared" si="2"/>
+        <v>0.39735099337748342</v>
+      </c>
+      <c r="V7" s="3">
+        <f>COUNTIF(D53:D201,0)+1</f>
+        <v>91</v>
+      </c>
+      <c r="W7" s="14">
+        <f t="shared" si="3"/>
+        <v>0.60264900662251653</v>
+      </c>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>32</v>
+      </c>
+      <c r="AC7" s="14">
+        <v>0.60377358490566035</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>21</v>
+      </c>
+      <c r="AE7" s="14">
+        <v>0.39622641509433965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="3">
+        <f>COUNTIF(E2:E52,1)+1</f>
+        <v>26</v>
+      </c>
+      <c r="Q8" s="14">
+        <f t="shared" si="0"/>
+        <v>0.49056603773584906</v>
+      </c>
+      <c r="R8" s="3">
+        <f>COUNTIF(E2:E52,0)+1</f>
+        <v>27</v>
+      </c>
+      <c r="S8" s="14">
+        <f t="shared" si="1"/>
+        <v>0.50943396226415094</v>
+      </c>
+      <c r="T8" s="3">
+        <f>COUNTIF(E53:E201,1)+1</f>
+        <v>51</v>
+      </c>
+      <c r="U8" s="14">
+        <f t="shared" si="2"/>
+        <v>0.33774834437086093</v>
+      </c>
+      <c r="V8" s="3">
+        <f>COUNTIF(E53:E201,0)+1</f>
+        <v>100</v>
+      </c>
+      <c r="W8" s="14">
+        <f t="shared" si="3"/>
+        <v>0.66225165562913912</v>
+      </c>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>26</v>
+      </c>
+      <c r="AC8" s="14">
+        <v>0.49056603773584906</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>27</v>
+      </c>
+      <c r="AE8" s="14">
+        <v>0.50943396226415094</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="3">
+        <f>COUNTIF(F2:F52,1)+1</f>
+        <v>19</v>
+      </c>
+      <c r="Q9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.35849056603773582</v>
+      </c>
+      <c r="R9" s="3">
+        <f>COUNTIF(F2:F52,0)+1</f>
+        <v>34</v>
+      </c>
+      <c r="S9" s="14">
+        <f t="shared" si="1"/>
+        <v>0.64150943396226412</v>
+      </c>
+      <c r="T9" s="3">
+        <f>COUNTIF(F53:F201,1)+1</f>
+        <v>71</v>
+      </c>
+      <c r="U9" s="14">
+        <f t="shared" si="2"/>
+        <v>0.47019867549668876</v>
+      </c>
+      <c r="V9" s="3">
+        <f>COUNTIF(F53:F201,0)+1</f>
+        <v>80</v>
+      </c>
+      <c r="W9" s="14">
+        <f t="shared" si="3"/>
+        <v>0.5298013245033113</v>
+      </c>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>19</v>
+      </c>
+      <c r="AC9" s="14">
+        <v>0.35849056603773582</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>34</v>
+      </c>
+      <c r="AE9" s="14">
+        <v>0.64150943396226412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="3">
+        <f>COUNTIF(G2:G52,1)+1</f>
+        <v>41</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" si="0"/>
+        <v>0.77358490566037741</v>
+      </c>
+      <c r="R10" s="3">
+        <f>COUNTIF(G2:G52,0)+1</f>
+        <v>12</v>
+      </c>
+      <c r="S10" s="14">
+        <f t="shared" si="1"/>
+        <v>0.22641509433962265</v>
+      </c>
+      <c r="T10" s="3">
+        <f>COUNTIF(G53:G201,1)+1</f>
+        <v>76</v>
+      </c>
+      <c r="U10" s="14">
+        <f t="shared" si="2"/>
+        <v>0.50331125827814571</v>
+      </c>
+      <c r="V10" s="3">
+        <f>COUNTIF(G53:G201,0)+1</f>
+        <v>75</v>
+      </c>
+      <c r="W10" s="14">
+        <f t="shared" si="3"/>
+        <v>0.49668874172185429</v>
+      </c>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>41</v>
+      </c>
+      <c r="AC10" s="14">
+        <v>0.77358490566037741</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>12</v>
+      </c>
+      <c r="AE10" s="14">
+        <v>0.22641509433962265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="3">
+        <f>COUNTIF(H2:H52,1)+1</f>
+        <v>40</v>
+      </c>
+      <c r="Q11" s="14">
+        <f t="shared" si="0"/>
+        <v>0.75471698113207553</v>
+      </c>
+      <c r="R11" s="3">
+        <f>COUNTIF(H2:H52,0)+1</f>
+        <v>13</v>
+      </c>
+      <c r="S11" s="14">
+        <f t="shared" si="1"/>
+        <v>0.24528301886792453</v>
+      </c>
+      <c r="T11" s="3">
+        <f>COUNTIF(H53:H201,1)+1</f>
+        <v>53</v>
+      </c>
+      <c r="U11" s="14">
+        <f t="shared" si="2"/>
+        <v>0.35099337748344372</v>
+      </c>
+      <c r="V11" s="3">
+        <f>COUNTIF(H53:H201,0)+1</f>
+        <v>98</v>
+      </c>
+      <c r="W11" s="14">
+        <f t="shared" si="3"/>
+        <v>0.64900662251655628</v>
+      </c>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>40</v>
+      </c>
+      <c r="AC11" s="14">
+        <v>0.75471698113207553</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>13</v>
+      </c>
+      <c r="AE11" s="14">
+        <v>0.24528301886792453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="3">
+        <f>COUNTIF(I2:I52,1)+1</f>
+        <v>18</v>
+      </c>
+      <c r="Q12" s="14">
+        <f t="shared" si="0"/>
+        <v>0.33962264150943394</v>
+      </c>
+      <c r="R12" s="3">
+        <f>COUNTIF(I2:I52,0)+1</f>
+        <v>35</v>
+      </c>
+      <c r="S12" s="14">
+        <f t="shared" si="1"/>
+        <v>0.660377358490566</v>
+      </c>
+      <c r="T12" s="3">
+        <f>COUNTIF(I53:I201,1)+1</f>
         <v>37</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3">
-        <f>COUNTIF(M2:M201,1)</f>
+      <c r="U12" s="14">
+        <f t="shared" si="2"/>
+        <v>0.24503311258278146</v>
+      </c>
+      <c r="V12" s="3">
+        <f>COUNTIF(I53:I201,0)+1</f>
+        <v>114</v>
+      </c>
+      <c r="W12" s="14">
+        <f t="shared" si="3"/>
+        <v>0.75496688741721851</v>
+      </c>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>18</v>
+      </c>
+      <c r="AC12" s="14">
+        <v>0.33962264150943394</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>35</v>
+      </c>
+      <c r="AE12" s="14">
+        <v>0.660377358490566</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" s="3">
+        <f>COUNTIF(J2:J52,1)+1</f>
+        <v>35</v>
+      </c>
+      <c r="Q13" s="14">
+        <f t="shared" si="0"/>
+        <v>0.660377358490566</v>
+      </c>
+      <c r="R13" s="3">
+        <f>COUNTIF(J2:J52,0)+1</f>
+        <v>18</v>
+      </c>
+      <c r="S13" s="14">
+        <f t="shared" si="1"/>
+        <v>0.33962264150943394</v>
+      </c>
+      <c r="T13" s="3">
+        <f>COUNTIF(J53:J201,1)+1</f>
+        <v>44</v>
+      </c>
+      <c r="U13" s="14">
+        <f t="shared" si="2"/>
+        <v>0.29139072847682118</v>
+      </c>
+      <c r="V13" s="3">
+        <f>COUNTIF(J53:J201,0)+1</f>
+        <v>107</v>
+      </c>
+      <c r="W13" s="14">
+        <f t="shared" si="3"/>
+        <v>0.70860927152317876</v>
+      </c>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>35</v>
+      </c>
+      <c r="AC13" s="14">
+        <v>0.660377358490566</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>18</v>
+      </c>
+      <c r="AE13" s="14">
+        <v>0.33962264150943394</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" s="3">
+        <f>COUNTIF(K2:K52,1)+1</f>
+        <v>35</v>
+      </c>
+      <c r="Q14" s="14">
+        <f t="shared" si="0"/>
+        <v>0.660377358490566</v>
+      </c>
+      <c r="R14" s="3">
+        <f>COUNTIF(K2:K52,0)+1</f>
+        <v>18</v>
+      </c>
+      <c r="S14" s="14">
+        <f t="shared" si="1"/>
+        <v>0.33962264150943394</v>
+      </c>
+      <c r="T14" s="3">
+        <f>COUNTIF(K53:K201,1)+1</f>
+        <v>88</v>
+      </c>
+      <c r="U14" s="14">
+        <f t="shared" si="2"/>
+        <v>0.58278145695364236</v>
+      </c>
+      <c r="V14" s="3">
+        <f>COUNTIF(K53:K201,0)+1</f>
+        <v>63</v>
+      </c>
+      <c r="W14" s="14">
+        <f t="shared" si="3"/>
+        <v>0.41721854304635764</v>
+      </c>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>35</v>
+      </c>
+      <c r="AC14" s="14">
+        <v>0.660377358490566</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>18</v>
+      </c>
+      <c r="AE14" s="14">
+        <v>0.33962264150943394</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" s="3">
+        <f>COUNTIF(L2:L52,1)+1</f>
+        <v>41</v>
+      </c>
+      <c r="Q15" s="14">
+        <f t="shared" si="0"/>
+        <v>0.77358490566037741</v>
+      </c>
+      <c r="R15" s="3">
+        <f>COUNTIF(L2:L52,0)+1</f>
+        <v>12</v>
+      </c>
+      <c r="S15" s="14">
+        <f t="shared" si="1"/>
+        <v>0.22641509433962265</v>
+      </c>
+      <c r="T15" s="3">
+        <f>COUNTIF(L53:L201,1)+1</f>
         <v>51</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3">
-        <f>COUNTIF(M2:M201,0)</f>
-        <v>149</v>
-      </c>
-      <c r="W3" s="3"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2" t="s">
+      <c r="U15" s="14">
+        <f t="shared" si="2"/>
+        <v>0.33774834437086093</v>
+      </c>
+      <c r="V15" s="3">
+        <f>COUNTIF(L53:L201,0)+1</f>
+        <v>100</v>
+      </c>
+      <c r="W15" s="14">
+        <f t="shared" si="3"/>
+        <v>0.66225165562913912</v>
+      </c>
+      <c r="Z15" s="20"/>
+      <c r="AA15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>41</v>
+      </c>
+      <c r="AC15" s="14">
+        <v>0.77358490566037741</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>12</v>
+      </c>
+      <c r="AE15" s="14">
+        <v>0.22641509433962265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q16" s="3">
+        <f>COUNTIF($M$2:$M$201,1)+1</f>
+        <v>52</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S16" s="14">
+        <f>Q16/(Q16+U16)</f>
+        <v>0.25742574257425743</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U16" s="3">
+        <f>COUNTIF($M$2:$M$201,0)+1</f>
+        <v>150</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W16" s="14">
+        <f>U16/(Q16+U16)</f>
+        <v>0.74257425742574257</v>
+      </c>
+      <c r="Z16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA16" s="4"/>
+      <c r="AB16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="2">
-        <f>COUNTIF(A2:A52,1)</f>
-        <v>34</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R4" s="2">
-        <f>COUNTIF(A2:A52,0)</f>
+      <c r="AE16" s="8"/>
+    </row>
+    <row r="17" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="16"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="16"/>
+      <c r="AA18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="4"/>
-      <c r="T4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" s="2">
-        <f>COUNTIF(A53:A201,1)</f>
+      <c r="AB18" s="3">
+        <v>54</v>
+      </c>
+      <c r="AC18" s="14">
+        <v>0.35761589403973509</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>97</v>
+      </c>
+      <c r="AE18" s="14">
+        <v>0.64238410596026485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="16"/>
+      <c r="AA19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>87</v>
+      </c>
+      <c r="AC19" s="14">
+        <v>0.57615894039735094</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>64</v>
+      </c>
+      <c r="AE19" s="14">
+        <v>0.42384105960264901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>52</v>
+      </c>
+      <c r="AC20" s="14">
+        <v>0.3443708609271523</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>99</v>
+      </c>
+      <c r="AE20" s="14">
+        <v>0.6556291390728477</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="16"/>
+      <c r="AA21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>60</v>
+      </c>
+      <c r="AC21" s="14">
+        <v>0.39735099337748342</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>91</v>
+      </c>
+      <c r="AE21" s="14">
+        <v>0.60264900662251653</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1</v>
+      </c>
+      <c r="M22" s="2">
+        <v>1</v>
+      </c>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Z22" s="16"/>
+      <c r="AA22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>51</v>
+      </c>
+      <c r="AC22" s="14">
+        <v>0.33774834437086093</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>100</v>
+      </c>
+      <c r="AE22" s="14">
+        <v>0.66225165562913912</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>71</v>
+      </c>
+      <c r="AC23" s="14">
+        <v>0.47019867549668876</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>80</v>
+      </c>
+      <c r="AE23" s="14">
+        <v>0.5298013245033113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1</v>
+      </c>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>76</v>
+      </c>
+      <c r="AC24" s="14">
+        <v>0.50331125827814571</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>75</v>
+      </c>
+      <c r="AE24" s="14">
+        <v>0.49668874172185429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>1</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1</v>
+      </c>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB25" s="3">
         <v>53</v>
       </c>
-      <c r="V4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="W4" s="2">
-        <f>COUNTIF(A53:A201,0)</f>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" s="2">
-        <f>COUNTIF(B2:B52,1)</f>
-        <v>30</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="2">
-        <f>COUNTIF(B2:B52,0)</f>
-        <v>21</v>
-      </c>
-      <c r="S5" s="4"/>
-      <c r="T5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="U5" s="2">
-        <f>COUNTIF(B53:B201,1)</f>
-        <v>86</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W5" s="2">
-        <f>COUNTIF(B53:B201,0)</f>
+      <c r="AC25" s="14">
+        <v>0.35099337748344372</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>98</v>
+      </c>
+      <c r="AE25" s="14">
+        <v>0.64900662251655628</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>1</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>37</v>
+      </c>
+      <c r="AC26" s="14">
+        <v>0.24503311258278146</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>114</v>
+      </c>
+      <c r="AE26" s="14">
+        <v>0.75496688741721851</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1</v>
+      </c>
+      <c r="M27" s="2">
+        <v>1</v>
+      </c>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>44</v>
+      </c>
+      <c r="AC27" s="14">
+        <v>0.29139072847682118</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>107</v>
+      </c>
+      <c r="AE27" s="14">
+        <v>0.70860927152317876</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1</v>
+      </c>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Z28" s="16"/>
+      <c r="AA28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>88</v>
+      </c>
+      <c r="AC28" s="14">
+        <v>0.58278145695364236</v>
+      </c>
+      <c r="AD28" s="3">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>0</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="2">
-        <f>COUNTIF(C2:C52,1)</f>
-        <v>23</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R6" s="2">
-        <f>COUNTIF(C2:C52,0)</f>
-        <v>28</v>
-      </c>
-      <c r="S6" s="4"/>
-      <c r="T6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U6" s="2">
-        <f>COUNTIF(C53:C201,1)</f>
+      <c r="AE28" s="14">
+        <v>0.41721854304635764</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB29" s="3">
         <v>51</v>
       </c>
-      <c r="V6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="W6" s="2">
-        <f>COUNTIF(C53:C201,0)</f>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
-        <v>0</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P7" s="2">
-        <f>COUNTIF(D2:D52,1)</f>
-        <v>31</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="2">
-        <f>COUNTIF(D2:D52,0)</f>
-        <v>20</v>
-      </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U7" s="2">
-        <f>COUNTIF(D53:D201,1)</f>
-        <v>59</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W7" s="2">
-        <f>COUNTIF(D53:D201,0)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8" s="2">
-        <f>COUNTIF(E2:E52,1)</f>
-        <v>25</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="2">
-        <f>COUNTIF(E2:E52,0)</f>
-        <v>26</v>
-      </c>
-      <c r="S8" s="4"/>
-      <c r="T8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U8" s="2">
-        <f>COUNTIF(E53:E201,1)</f>
+      <c r="AC29" s="14">
+        <v>0.33774834437086093</v>
+      </c>
+      <c r="AD29" s="3">
+        <v>100</v>
+      </c>
+      <c r="AE29" s="14">
+        <v>0.66225165562913912</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>1</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1</v>
+      </c>
+      <c r="M30" s="2">
+        <v>1</v>
+      </c>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="8"/>
+      <c r="AB30" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="V8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="W8" s="2">
-        <f>COUNTIF(E53:E201,0)</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="2">
-        <f>COUNTIF(F2:F52,1)</f>
-        <v>18</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" s="2">
-        <f>COUNTIF(F2:F52,0)</f>
-        <v>33</v>
-      </c>
-      <c r="S9" s="4"/>
-      <c r="T9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" s="2">
-        <f>COUNTIF(F53:F201,1)</f>
-        <v>70</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="W9" s="2">
-        <f>COUNTIF(F53:F201,0)</f>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="2">
-        <f>COUNTIF(G2:G52,1)</f>
-        <v>40</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R10" s="2">
-        <f>COUNTIF(G2:G52,0)</f>
-        <v>11</v>
-      </c>
-      <c r="S10" s="4"/>
-      <c r="T10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U10" s="2">
-        <f>COUNTIF(G53:G201,1)</f>
-        <v>75</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W10" s="2">
-        <f>COUNTIF(G53:G201,0)</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="2">
-        <v>1</v>
-      </c>
-      <c r="M11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P11" s="2">
-        <f>COUNTIF(H2:H52,1)</f>
-        <v>39</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="R11" s="2">
-        <f>COUNTIF(H2:H52,0)</f>
-        <v>12</v>
-      </c>
-      <c r="S11" s="4"/>
-      <c r="T11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U11" s="2">
-        <f>COUNTIF(H53:H201,1)</f>
+      <c r="AC30" s="4"/>
+      <c r="AD30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE30" s="4"/>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="M31" s="2">
+        <v>1</v>
+      </c>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Z31" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA31" s="4"/>
+      <c r="AB31" s="6">
         <v>52</v>
       </c>
-      <c r="V11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W11" s="2">
-        <f>COUNTIF(H53:H201,0)</f>
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P12" s="2">
-        <f>COUNTIF(I2:I52,1)</f>
-        <v>17</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R12" s="2">
-        <f>COUNTIF(I2:I52,0)</f>
-        <v>34</v>
-      </c>
-      <c r="S12" s="4"/>
-      <c r="T12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U12" s="2">
-        <f>COUNTIF(I53:I201,1)</f>
-        <v>36</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W12" s="2">
-        <f>COUNTIF(I53:I201,0)</f>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P13" s="2">
-        <f>COUNTIF(J2:J52,1)</f>
-        <v>34</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R13" s="2">
-        <f>COUNTIF(J2:J52,0)</f>
-        <v>17</v>
-      </c>
-      <c r="S13" s="4"/>
-      <c r="T13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U13" s="2">
-        <f>COUNTIF(J53:J201,1)</f>
+      <c r="AC31" s="8"/>
+      <c r="AD31" s="21">
+        <v>0.25742574257425699</v>
+      </c>
+      <c r="AE31" s="22"/>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1</v>
+      </c>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Z32" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="W13" s="2">
-        <f>COUNTIF(J53:J201,0)</f>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>0</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" s="2">
-        <f>COUNTIF(K2:K52,1)</f>
-        <v>34</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R14" s="2">
-        <f>COUNTIF(K2:K52,0)</f>
-        <v>17</v>
-      </c>
-      <c r="S14" s="4"/>
-      <c r="T14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U14" s="2">
-        <f>COUNTIF(K53:K201,1)</f>
-        <v>87</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="W14" s="2">
-        <f>COUNTIF(K53:K201,0)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-      <c r="M15" s="2">
-        <v>1</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="2">
-        <f>COUNTIF(L2:L52,1)</f>
-        <v>40</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R15" s="2">
-        <f>COUNTIF(L2:L52,0)</f>
-        <v>11</v>
-      </c>
-      <c r="S15" s="4"/>
-      <c r="T15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U15" s="2">
-        <f>COUNTIF(L53:L201,1)</f>
-        <v>50</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W15" s="2">
-        <f>COUNTIF(L53:L201,0)</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <v>0</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2">
-        <v>1</v>
-      </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1</v>
-      </c>
-      <c r="J17" s="2">
-        <v>1</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2">
-        <v>1</v>
-      </c>
-      <c r="M17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>0</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1</v>
-      </c>
-      <c r="L18" s="2">
-        <v>1</v>
-      </c>
-      <c r="M18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2">
-        <v>1</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0</v>
-      </c>
-      <c r="K19" s="2">
-        <v>1</v>
-      </c>
-      <c r="L19" s="2">
-        <v>1</v>
-      </c>
-      <c r="M19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0</v>
-      </c>
-      <c r="K20" s="2">
-        <v>1</v>
-      </c>
-      <c r="L20" s="2">
-        <v>1</v>
-      </c>
-      <c r="M20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2">
-        <v>0</v>
-      </c>
-      <c r="L21" s="2">
-        <v>1</v>
-      </c>
-      <c r="M21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2">
-        <v>1</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1</v>
-      </c>
-      <c r="L22" s="2">
-        <v>1</v>
-      </c>
-      <c r="M22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>1</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0</v>
-      </c>
-      <c r="L23" s="2">
-        <v>1</v>
-      </c>
-      <c r="M23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <v>0</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2">
-        <v>1</v>
-      </c>
-      <c r="H24" s="2">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>1</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
-      <c r="L24" s="2">
-        <v>1</v>
-      </c>
-      <c r="M24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-      <c r="H25" s="2">
-        <v>1</v>
-      </c>
-      <c r="I25" s="2">
-        <v>1</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0</v>
-      </c>
-      <c r="K25" s="2">
-        <v>1</v>
-      </c>
-      <c r="L25" s="2">
-        <v>1</v>
-      </c>
-      <c r="M25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>1</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1</v>
-      </c>
-      <c r="H26" s="2">
-        <v>1</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0</v>
-      </c>
-      <c r="K26" s="2">
-        <v>1</v>
-      </c>
-      <c r="L26" s="2">
-        <v>1</v>
-      </c>
-      <c r="M26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>0</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <v>1</v>
-      </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2">
-        <v>1</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
-        <v>0</v>
-      </c>
-      <c r="J27" s="2">
-        <v>1</v>
-      </c>
-      <c r="K27" s="2">
-        <v>0</v>
-      </c>
-      <c r="L27" s="2">
-        <v>1</v>
-      </c>
-      <c r="M27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>0</v>
-      </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0</v>
-      </c>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2">
-        <v>1</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0</v>
-      </c>
-      <c r="K28" s="2">
-        <v>1</v>
-      </c>
-      <c r="L28" s="2">
-        <v>1</v>
-      </c>
-      <c r="M28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>0</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <v>0</v>
-      </c>
-      <c r="J29" s="2">
-        <v>1</v>
-      </c>
-      <c r="K29" s="2">
-        <v>1</v>
-      </c>
-      <c r="L29" s="2">
-        <v>1</v>
-      </c>
-      <c r="M29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>1</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1</v>
-      </c>
-      <c r="I30" s="2">
-        <v>1</v>
-      </c>
-      <c r="J30" s="2">
-        <v>1</v>
-      </c>
-      <c r="K30" s="2">
-        <v>0</v>
-      </c>
-      <c r="L30" s="2">
-        <v>1</v>
-      </c>
-      <c r="M30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
-        <v>0</v>
-      </c>
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0</v>
-      </c>
-      <c r="F31" s="2">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <v>1</v>
-      </c>
-      <c r="J31" s="2">
-        <v>0</v>
-      </c>
-      <c r="K31" s="2">
-        <v>1</v>
-      </c>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
-      <c r="M31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2">
-        <v>1</v>
-      </c>
-      <c r="K32" s="2">
-        <v>1</v>
-      </c>
-      <c r="L32" s="2">
-        <v>1</v>
-      </c>
-      <c r="M32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="AA32" s="4"/>
+      <c r="AB32" s="6">
+        <v>150</v>
+      </c>
+      <c r="AC32" s="8"/>
+      <c r="AD32" s="21">
+        <v>0.74257425742574301</v>
+      </c>
+      <c r="AE32" s="22"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -2868,8 +3518,12 @@
       <c r="M33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -2909,8 +3563,12 @@
       <c r="M34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>1</v>
       </c>
@@ -2950,8 +3608,12 @@
       <c r="M35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -2991,8 +3653,12 @@
       <c r="M36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>0</v>
       </c>
@@ -3032,8 +3698,12 @@
       <c r="M37" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>0</v>
       </c>
@@ -3073,8 +3743,12 @@
       <c r="M38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -3114,8 +3788,12 @@
       <c r="M39" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>1</v>
       </c>
@@ -3155,8 +3833,12 @@
       <c r="M40" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>1</v>
       </c>
@@ -3197,7 +3879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -3238,7 +3920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>1</v>
       </c>
@@ -3279,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>1</v>
       </c>
@@ -3320,7 +4002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>1</v>
       </c>
@@ -3361,7 +4043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>1</v>
       </c>
@@ -3402,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>1</v>
       </c>
@@ -3443,7 +4125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>0</v>
       </c>
@@ -9758,13 +10440,33 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
+  <mergeCells count="24">
+    <mergeCell ref="Z31:AA31"/>
+    <mergeCell ref="Z32:AA32"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AD30:AE30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="AB31:AC31"/>
+    <mergeCell ref="AB32:AC32"/>
+    <mergeCell ref="AD31:AE31"/>
+    <mergeCell ref="AD32:AE32"/>
+    <mergeCell ref="Z2:Z15"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="Z16:Z29"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AB16:AC16"/>
+    <mergeCell ref="AD16:AE16"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>